<commit_message>
Snowing pretty hard so stopping. Updated Matcher to support chaining and matching by property path through reflection. Also implmented trigger types and added an images matcher
</commit_message>
<xml_diff>
--- a/MatcherNotes.xlsx
+++ b/MatcherNotes.xlsx
@@ -4,8 +4,9 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-9" yWindow="-9" windowWidth="24720" windowHeight="4371"/>
-    <workbookView xWindow="-9" yWindow="4440" windowWidth="24720" windowHeight="7714" activeTab="1"/>
+    <workbookView xWindow="9" yWindow="-43" windowWidth="24720" windowHeight="4226" activeTab="2"/>
+    <workbookView xWindow="17" yWindow="7860" windowWidth="24720" windowHeight="4286" activeTab="1"/>
+    <workbookView xWindow="51" yWindow="4097" windowWidth="24549" windowHeight="3891"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,11 +14,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="68">
   <si>
     <t>Triggers</t>
   </si>
@@ -52,15 +54,9 @@
     <t>Matcher</t>
   </si>
   <si>
-    <t>Trigger</t>
-  </si>
-  <si>
     <t>Trigger Action</t>
   </si>
   <si>
-    <t>Match Reaction</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -82,32 +78,158 @@
     <t>TagId</t>
   </si>
   <si>
-    <t>ShortcutId</t>
-  </si>
-  <si>
     <t>Shortcut.CommandId</t>
   </si>
   <si>
-    <t>Trigger(Type,Id,Args)</t>
-  </si>
-  <si>
     <t>Examples</t>
   </si>
   <si>
-    <t>IsMatch Reaction</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>When image is copied it is added to tag 'Images'</t>
+  </si>
+  <si>
+    <t>IsMatchPropertyPath</t>
+  </si>
+  <si>
+    <t>Match Data</t>
+  </si>
+  <si>
+    <t>ItemType</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Match Action (Type,ObjId,Args)</t>
+  </si>
+  <si>
+    <t>Trigger Action (Type,ObjId,Args)</t>
+  </si>
+  <si>
+    <t>Trigger Type</t>
+  </si>
+  <si>
+    <t>CopyItemId (User Selected)</t>
+  </si>
+  <si>
+    <t>ParentMatcherId (or 0)</t>
+  </si>
+  <si>
+    <t>AnalyiticItemId</t>
+  </si>
+  <si>
+    <t>When image is copied from facebook.com and has cat in it add it to tag 'Cats'</t>
+  </si>
+  <si>
+    <t>ParentMatchOutput</t>
+  </si>
+  <si>
+    <t>MatcherId</t>
+  </si>
+  <si>
+    <t>Source.PrimarySource.UrlPath</t>
+  </si>
+  <si>
+    <t>facebook.com</t>
+  </si>
+  <si>
+    <t>(AnalyzerResultCopyItemId).ItemData</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>Compare</t>
+  </si>
+  <si>
+    <t>SortOrderIdx</t>
+  </si>
+  <si>
+    <t>User adds image to 'Mobile Asset' Tag and image is transformed into 16x16,32x32,64x64 resolution .pngs into '…/Assets/&lt;ImageItemTitle&gt;_&lt;W&gt;x&lt;H&gt;.png</t>
+  </si>
+  <si>
+    <t>CopyItemId (FileList Type, Directory Path)</t>
+  </si>
+  <si>
+    <t>Transform (16x16 path)</t>
+  </si>
+  <si>
+    <t>Transform (32x32 path)</t>
+  </si>
+  <si>
+    <t>Transform (64x64 path)</t>
+  </si>
+  <si>
+    <t>User copies webpage html and is added to 'Html','JavaScript' and 'Css' tags</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>ItemData</t>
+  </si>
+  <si>
+    <t>Html(Regex or 'bool IsMatch(string input)' dynamic method)</t>
+  </si>
+  <si>
+    <t>Javascript(Regex or 'bool IsMatch(string input)' dynamic method)</t>
+  </si>
+  <si>
+    <t>Css (Regex or 'bool IsMatch(string input)' dynamic method)</t>
+  </si>
+  <si>
+    <t>MpMatchTriggerType</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>ContentItemAdded</t>
+  </si>
+  <si>
+    <t>WatchFileChanged</t>
+  </si>
+  <si>
+    <t>WatchFolderChange</t>
+  </si>
+  <si>
+    <t>ContentItemAddedToTag</t>
+  </si>
+  <si>
+    <t>Shortcut</t>
+  </si>
+  <si>
+    <t>MpMatchActionType</t>
+  </si>
+  <si>
+    <t>MpMatcherType</t>
+  </si>
+  <si>
+    <t>Contains</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>BeginsWith</t>
+  </si>
+  <si>
+    <t>EndsWith</t>
+  </si>
+  <si>
+    <t>RegEx</t>
+  </si>
+  <si>
+    <t>Source</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,8 +260,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +294,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -177,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -191,6 +357,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,132 +703,178 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM13"/>
+  <dimension ref="A1:AN13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="I1" sqref="I1:M3"/>
-    </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
     <col min="1" max="1" width="18.53515625" customWidth="1"/>
-    <col min="2" max="2" width="22.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.3046875" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="11.23046875" customWidth="1"/>
+    <col min="4" max="4" width="3.3828125" style="7" customWidth="1"/>
     <col min="5" max="6" width="17.61328125" customWidth="1"/>
-    <col min="8" max="8" width="23.23046875" customWidth="1"/>
+    <col min="7" max="7" width="42.07421875" customWidth="1"/>
+    <col min="8" max="8" width="3.3046875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="33.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="1" customFormat="1" ht="31.3" customHeight="1">
+    <row r="1" spans="1:40" s="1" customFormat="1" ht="31.3" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D1" s="7"/>
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7"/>
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:39" s="3" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:40" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="D2" s="7"/>
       <c r="E2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:39">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:40">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:39">
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:39">
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:39">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:39">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:39" s="2" customFormat="1" ht="22.3" customHeight="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" s="2" customFormat="1" ht="22.3" customHeight="1">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
-      <c r="D11"/>
+      <c r="D11" s="7"/>
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
-      <c r="H11"/>
+      <c r="H11" s="7"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -642,16 +906,17 @@
       <c r="AK11"/>
       <c r="AL11"/>
       <c r="AM11"/>
-    </row>
-    <row r="12" spans="1:39" s="3" customFormat="1">
+      <c r="AN11"/>
+    </row>
+    <row r="12" spans="1:40" s="3" customFormat="1">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
-      <c r="D12"/>
+      <c r="D12" s="7"/>
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12"/>
-      <c r="H12"/>
+      <c r="H12" s="7"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -683,11 +948,14 @@
       <c r="AK12"/>
       <c r="AL12"/>
       <c r="AM12"/>
-    </row>
-    <row r="13" spans="1:39" s="5" customFormat="1" ht="55.75" customHeight="1">
+      <c r="AN12"/>
+    </row>
+    <row r="13" spans="1:40" s="5" customFormat="1" ht="55.75" customHeight="1">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
+      <c r="D13" s="7"/>
+      <c r="H13" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -697,56 +965,368 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="1">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView showRowColHeaders="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="19.765625" customWidth="1"/>
-    <col min="2" max="2" width="16.4609375" customWidth="1"/>
-    <col min="3" max="3" width="17.15234375" customWidth="1"/>
-    <col min="4" max="4" width="15.3828125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.765625" customWidth="1"/>
+    <col min="1" max="1" width="17.3828125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="19.765625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="27.4609375" style="17" customWidth="1"/>
+    <col min="4" max="4" width="34.921875" style="17" customWidth="1"/>
+    <col min="5" max="5" width="27.3828125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="37.07421875" customWidth="1"/>
+    <col min="7" max="12" width="9.23046875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" ht="18.45">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="18.45">
+      <c r="A1" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+    </row>
+    <row r="2" spans="1:12" s="3" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="3" customFormat="1">
-      <c r="A2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+    </row>
+    <row r="3" spans="1:12" ht="29.15">
+      <c r="A3" s="21">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="87.45">
-      <c r="A3" s="5" t="s">
+      <c r="F3" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="16.3" customHeight="1">
+      <c r="A4" s="21">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" ht="24" customHeight="1">
+      <c r="A5" s="19"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:12" ht="48" customHeight="1">
+      <c r="A6" s="21">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="40.299999999999997" customHeight="1">
+      <c r="A7" s="21">
+        <v>0</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:12" ht="31.75" customHeight="1">
+      <c r="A8" s="21">
+        <v>0</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="21">
+        <v>0</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="19"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:12" ht="77.599999999999994" customHeight="1">
+      <c r="A11" s="21">
+        <v>0</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="35.6" customHeight="1">
+      <c r="A12" s="21">
+        <v>0</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="21">
+        <v>1</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="21">
+        <v>2</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+    </row>
+    <row r="16" spans="1:12" ht="29.15">
+      <c r="A16" s="21">
+        <v>0</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="43.75">
+      <c r="A17" s="21">
+        <v>0</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="21">
+        <v>0</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="1:6" ht="43.75">
+      <c r="A19" s="21">
+        <v>1</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="21">
+        <v>0</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:6" ht="43.75">
+      <c r="A21" s="21">
+        <v>2</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="21">
+        <v>0</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -756,13 +1336,171 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
     <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="18.45"/>
+  <cols>
+    <col min="1" max="1" width="24.23046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.69140625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="23.61328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.15234375" style="11" customWidth="1"/>
+    <col min="8" max="8" width="14.765625" customWidth="1"/>
+    <col min="9" max="9" width="9.23046875" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="4" customFormat="1">
+      <c r="A1" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="23"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="26"/>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16.3" customHeight="1">
+      <c r="A3" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="5">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="5">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="5">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="5">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed bug copying image from web where html is different than copying text. Added MonkeyPaste.Plugin project and made use case project dependent on it. Created MpIMatchTrigger interface for trigger actions. Also added Autofac back and am about to remove singleton stuff and use IoC instead.
</commit_message>
<xml_diff>
--- a/MatcherNotes.xlsx
+++ b/MatcherNotes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="69">
   <si>
     <t>Triggers</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>Source</t>
+  </si>
+  <si>
+    <t>Automatic</t>
   </si>
 </sst>
 </file>
@@ -709,7 +712,9 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView tabSelected="1" workbookViewId="2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="2">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
@@ -969,7 +974,7 @@
   <sheetViews>
     <sheetView showRowColHeaders="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
     <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
     <sheetView workbookViewId="2"/>
   </sheetViews>
@@ -1336,10 +1341,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
     <sheetView workbookViewId="2"/>
@@ -1388,7 +1393,7 @@
         <v>54</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16.3" customHeight="1">
@@ -1408,7 +1413,7 @@
         <v>62</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1428,7 +1433,7 @@
         <v>63</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1448,7 +1453,7 @@
         <v>64</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1468,7 +1473,7 @@
         <v>65</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1482,7 +1487,7 @@
         <v>66</v>
       </c>
       <c r="H7">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1496,7 +1501,15 @@
         <v>67</v>
       </c>
       <c r="H8">
-        <v>6</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="G9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working through action trere view initialization and template binding complexities. Also ucrtbase.dll bug is back...Brough back my old timer based monitor that worked and have that in seperate project now so hopefully that resolves the issue.
</commit_message>
<xml_diff>
--- a/MatcherNotes.xlsx
+++ b/MatcherNotes.xlsx
@@ -4,9 +4,9 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="9" yWindow="-43" windowWidth="24720" windowHeight="4226" activeTab="2"/>
-    <workbookView xWindow="17" yWindow="7860" windowWidth="24720" windowHeight="4286" activeTab="1"/>
-    <workbookView xWindow="51" yWindow="4097" windowWidth="24549" windowHeight="3891"/>
+    <workbookView xWindow="9" yWindow="-43" windowWidth="24720" windowHeight="4714" activeTab="2"/>
+    <workbookView xWindow="17" yWindow="4834" windowWidth="24720" windowHeight="7311" activeTab="1"/>
+    <workbookView xWindow="51" yWindow="4097" windowWidth="24549" windowHeight="1123"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="82">
   <si>
     <t>Triggers</t>
   </si>
@@ -54,9 +53,6 @@
     <t>Matcher</t>
   </si>
   <si>
-    <t>Trigger Action</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -90,12 +86,6 @@
     <t>When image is copied it is added to tag 'Images'</t>
   </si>
   <si>
-    <t>IsMatchPropertyPath</t>
-  </si>
-  <si>
-    <t>Match Data</t>
-  </si>
-  <si>
     <t>ItemType</t>
   </si>
   <si>
@@ -180,9 +170,6 @@
     <t>Css (Regex or 'bool IsMatch(string input)' dynamic method)</t>
   </si>
   <si>
-    <t>MpMatchTriggerType</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -201,12 +188,6 @@
     <t>Shortcut</t>
   </si>
   <si>
-    <t>MpMatchActionType</t>
-  </si>
-  <si>
-    <t>MpMatcherType</t>
-  </si>
-  <si>
     <t>Contains</t>
   </si>
   <si>
@@ -226,13 +207,70 @@
   </si>
   <si>
     <t>Automatic</t>
+  </si>
+  <si>
+    <t>Macro</t>
+  </si>
+  <si>
+    <t>Paste Special</t>
+  </si>
+  <si>
+    <t>User right clicks a pdf file list item where in the Transform menu a "To DocX" option is dynamically available and clicked so new item is inserted below pdf as docx</t>
+  </si>
+  <si>
+    <t>FileList</t>
+  </si>
+  <si>
+    <t>ParentId</t>
+  </si>
+  <si>
+    <t>Action Type</t>
+  </si>
+  <si>
+    <t>MpActionType</t>
+  </si>
+  <si>
+    <t>MpTriggerType</t>
+  </si>
+  <si>
+    <t>Arg1</t>
+  </si>
+  <si>
+    <t>Arg2</t>
+  </si>
+  <si>
+    <t>Arg3</t>
+  </si>
+  <si>
+    <t>.pdf</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>Property Path</t>
+  </si>
+  <si>
+    <t>MpCompareType</t>
+  </si>
+  <si>
+    <t>CompareType</t>
+  </si>
+  <si>
+    <t>Compare Data</t>
+  </si>
+  <si>
+    <t>Command Obj Type</t>
+  </si>
+  <si>
+    <t>Command Obj Id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,8 +309,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,6 +378,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -346,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -378,9 +429,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -412,6 +460,14 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -743,23 +799,23 @@
     </row>
     <row r="2" spans="1:40" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="G2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="7"/>
     </row>
@@ -768,22 +824,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:40">
@@ -791,22 +847,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:40">
@@ -814,19 +870,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:40">
@@ -834,19 +890,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:40">
@@ -854,21 +910,21 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:40">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:40" s="2" customFormat="1" ht="22.3" customHeight="1">
@@ -970,368 +1026,869 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:O97"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
     <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
     <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="17.3828125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="19.765625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="27.4609375" style="17" customWidth="1"/>
-    <col min="4" max="4" width="34.921875" style="17" customWidth="1"/>
-    <col min="5" max="5" width="27.3828125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="37.07421875" customWidth="1"/>
-    <col min="7" max="12" width="9.23046875" style="11"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="17.3828125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="19.765625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="27.4609375" style="16" customWidth="1"/>
+    <col min="6" max="6" width="34.921875" style="16" customWidth="1"/>
+    <col min="7" max="7" width="27.3828125" style="16" customWidth="1"/>
+    <col min="8" max="8" width="17.69140625" style="16" customWidth="1"/>
+    <col min="9" max="9" width="37.07421875" customWidth="1"/>
+    <col min="10" max="15" width="9.23046875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="18.45">
-      <c r="A1" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+    <row r="1" spans="1:15" s="4" customFormat="1" ht="18.45">
+      <c r="A1" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
-    </row>
-    <row r="2" spans="1:12" s="3" customFormat="1">
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+    </row>
+    <row r="2" spans="1:15" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+        <v>71</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
-    </row>
-    <row r="3" spans="1:12" ht="29.15">
-      <c r="A3" s="21">
-        <v>0</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>40</v>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+    </row>
+    <row r="3" spans="1:15" ht="29.15">
+      <c r="A3" s="20">
+        <v>1</v>
+      </c>
+      <c r="B3" s="20">
+        <v>0</v>
+      </c>
+      <c r="C3" s="20">
+        <v>0</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="16.3" customHeight="1">
-      <c r="A4" s="21">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="G3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="16.3" customHeight="1">
+      <c r="A4" s="20">
+        <v>2</v>
+      </c>
+      <c r="B4" s="20">
+        <v>1</v>
+      </c>
+      <c r="C4" s="20">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
-    </row>
-    <row r="5" spans="1:12" ht="24" customHeight="1">
-      <c r="A5" s="19"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:15" ht="24" customHeight="1">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
-    </row>
-    <row r="6" spans="1:12" ht="48" customHeight="1">
-      <c r="A6" s="21">
-        <v>0</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>40</v>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" spans="1:15" ht="48" customHeight="1">
+      <c r="A6" s="20">
+        <v>1</v>
+      </c>
+      <c r="B6" s="20">
+        <v>0</v>
+      </c>
+      <c r="C6" s="20">
+        <v>0</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="25.75" customHeight="1">
+      <c r="A7" s="20">
+        <v>2</v>
+      </c>
+      <c r="B7" s="20">
+        <v>1</v>
+      </c>
+      <c r="C7" s="20">
+        <v>0</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="16" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="40.299999999999997" customHeight="1">
-      <c r="A7" s="21">
-        <v>0</v>
-      </c>
-      <c r="B7" s="17" t="s">
+      <c r="G7" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="17" t="s">
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="1:15" ht="23.15" customHeight="1">
+      <c r="A8" s="20">
+        <v>3</v>
+      </c>
+      <c r="B8" s="20">
+        <v>2</v>
+      </c>
+      <c r="C8" s="20">
+        <v>0</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:12" ht="31.75" customHeight="1">
-      <c r="A8" s="21">
-        <v>0</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="21">
-        <v>0</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="17" t="s">
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="20">
+        <v>4</v>
+      </c>
+      <c r="B9" s="20">
+        <v>3</v>
+      </c>
+      <c r="C9" s="20">
+        <v>0</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
       <c r="F9" s="8"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="19"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="14"/>
-    </row>
-    <row r="11" spans="1:12" ht="77.599999999999994" customHeight="1">
-      <c r="A11" s="21">
-        <v>0</v>
-      </c>
-      <c r="B11" s="17" t="s">
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="14"/>
+    </row>
+    <row r="11" spans="1:15" ht="77.599999999999994" customHeight="1">
+      <c r="A11" s="20">
+        <v>1</v>
+      </c>
+      <c r="B11" s="20">
+        <v>0</v>
+      </c>
+      <c r="C11" s="20">
+        <v>0</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="E11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="35.6" customHeight="1">
+      <c r="A12" s="20">
+        <v>2</v>
+      </c>
+      <c r="B12" s="20">
+        <v>1</v>
+      </c>
+      <c r="C12" s="20">
+        <v>0</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+    </row>
+    <row r="13" spans="1:15" ht="22.75" customHeight="1">
+      <c r="A13" s="20">
+        <v>3</v>
+      </c>
+      <c r="B13" s="20">
+        <v>1</v>
+      </c>
+      <c r="C13" s="20">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="16" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="35.6" customHeight="1">
-      <c r="A12" s="21">
-        <v>0</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="21">
-        <v>1</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
       <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="21">
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="20">
+        <v>4</v>
+      </c>
+      <c r="B14" s="20">
+        <v>1</v>
+      </c>
+      <c r="C14" s="20">
         <v>2</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="D14" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>43</v>
+      </c>
       <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-    </row>
-    <row r="16" spans="1:12" ht="29.15">
-      <c r="A16" s="21">
-        <v>0</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>40</v>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+    </row>
+    <row r="16" spans="1:15" ht="29.15">
+      <c r="A16" s="20">
+        <v>1</v>
+      </c>
+      <c r="B16" s="20">
+        <v>0</v>
+      </c>
+      <c r="C16" s="20">
+        <v>0</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="5"/>
+      <c r="I16" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="43.75">
+      <c r="A17" s="20">
+        <v>2</v>
+      </c>
+      <c r="B17" s="20">
+        <v>1</v>
+      </c>
+      <c r="C17" s="20">
+        <v>0</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="20">
+        <v>3</v>
+      </c>
+      <c r="B18" s="20">
+        <v>2</v>
+      </c>
+      <c r="C18" s="20">
+        <v>0</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+    </row>
+    <row r="19" spans="1:9" ht="43.75">
+      <c r="A19" s="20">
+        <v>4</v>
+      </c>
+      <c r="B19" s="20">
+        <v>1</v>
+      </c>
+      <c r="C19" s="20">
+        <v>1</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="43.75">
-      <c r="A17" s="21">
-        <v>0</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="17" t="s">
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="20">
+        <v>5</v>
+      </c>
+      <c r="B20" s="20">
+        <v>4</v>
+      </c>
+      <c r="C20" s="20">
+        <v>0</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="1:9" ht="43.75">
+      <c r="A21" s="20">
+        <v>6</v>
+      </c>
+      <c r="B21" s="20">
+        <v>1</v>
+      </c>
+      <c r="C21" s="20">
+        <v>2</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="21">
-        <v>0</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="17" t="s">
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="20">
         <v>7</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:6" ht="43.75">
-      <c r="A19" s="21">
-        <v>1</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="21">
-        <v>0</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="17" t="s">
+      <c r="B22" s="20">
+        <v>6</v>
+      </c>
+      <c r="C22" s="20">
+        <v>0</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="1:6" ht="43.75">
-      <c r="A21" s="21">
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+    </row>
+    <row r="24" spans="1:9" ht="62.6" customHeight="1">
+      <c r="A24" s="20">
+        <v>1</v>
+      </c>
+      <c r="B24" s="20">
+        <v>0</v>
+      </c>
+      <c r="C24" s="20">
+        <v>0</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="20">
         <v>2</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="21">
-        <v>0</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
+      <c r="B25" s="20">
+        <v>1</v>
+      </c>
+      <c r="C25" s="20">
+        <v>0</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="20">
+        <v>3</v>
+      </c>
+      <c r="B26" s="20">
+        <v>2</v>
+      </c>
+      <c r="C26" s="20">
+        <v>0</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="20"/>
+      <c r="B31" s="20"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="20"/>
+      <c r="B32" s="20"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="20"/>
+      <c r="B33" s="20"/>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="20"/>
+      <c r="B34" s="20"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="20"/>
+      <c r="B35" s="20"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="20"/>
+      <c r="B36" s="20"/>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="20"/>
+      <c r="B37" s="20"/>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="20"/>
+      <c r="B38" s="20"/>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="20"/>
+      <c r="B39" s="20"/>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="20"/>
+      <c r="B40" s="20"/>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="20"/>
+      <c r="B41" s="20"/>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="20"/>
+      <c r="B42" s="20"/>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="20"/>
+      <c r="B43" s="20"/>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="20"/>
+      <c r="B44" s="20"/>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="20"/>
+      <c r="B45" s="20"/>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="20"/>
+      <c r="B46" s="20"/>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="20"/>
+      <c r="B47" s="20"/>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="20"/>
+      <c r="B48" s="20"/>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="20"/>
+      <c r="B49" s="20"/>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="20"/>
+      <c r="B50" s="20"/>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="20"/>
+      <c r="B51" s="20"/>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="20"/>
+      <c r="B52" s="20"/>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="20"/>
+      <c r="B53" s="20"/>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="20"/>
+      <c r="B54" s="20"/>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="20"/>
+      <c r="B55" s="20"/>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="20"/>
+      <c r="B56" s="20"/>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="20"/>
+      <c r="B57" s="20"/>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="20"/>
+      <c r="B58" s="20"/>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="20"/>
+      <c r="B59" s="20"/>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="20"/>
+      <c r="B60" s="20"/>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="20"/>
+      <c r="B61" s="20"/>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="20"/>
+      <c r="B62" s="20"/>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="20"/>
+      <c r="B63" s="20"/>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="20"/>
+      <c r="B64" s="20"/>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="20"/>
+      <c r="B65" s="20"/>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="20"/>
+      <c r="B66" s="20"/>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="20"/>
+      <c r="B67" s="20"/>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="20"/>
+      <c r="B68" s="20"/>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="20"/>
+      <c r="B69" s="20"/>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="20"/>
+      <c r="B70" s="20"/>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="20"/>
+      <c r="B71" s="20"/>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="20"/>
+      <c r="B72" s="20"/>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="20"/>
+      <c r="B73" s="20"/>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="20"/>
+      <c r="B74" s="20"/>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="20"/>
+      <c r="B75" s="20"/>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="20"/>
+      <c r="B76" s="20"/>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="20"/>
+      <c r="B77" s="20"/>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="20"/>
+      <c r="B78" s="20"/>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="20"/>
+      <c r="B79" s="20"/>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="20"/>
+      <c r="B80" s="20"/>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="20"/>
+      <c r="B81" s="20"/>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="20"/>
+      <c r="B82" s="20"/>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="20"/>
+      <c r="B83" s="20"/>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="20"/>
+      <c r="B84" s="20"/>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="20"/>
+      <c r="B85" s="20"/>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="20"/>
+      <c r="B86" s="20"/>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="20"/>
+      <c r="B87" s="20"/>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="20"/>
+      <c r="B88" s="20"/>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="20"/>
+      <c r="B89" s="20"/>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="20"/>
+      <c r="B90" s="20"/>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="20"/>
+      <c r="B91" s="20"/>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="20"/>
+      <c r="B92" s="20"/>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="20"/>
+      <c r="B93" s="20"/>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="20"/>
+      <c r="B94" s="20"/>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="20"/>
+      <c r="B95" s="20"/>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="20"/>
+      <c r="B96" s="20"/>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="20"/>
+      <c r="B97" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1341,10 +1898,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
     <sheetView workbookViewId="2"/>
@@ -1354,163 +1911,257 @@
     <col min="1" max="1" width="24.23046875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.69140625" style="10" customWidth="1"/>
     <col min="4" max="4" width="23.61328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.23046875" style="26"/>
     <col min="6" max="6" width="2.15234375" style="11" customWidth="1"/>
-    <col min="8" max="8" width="14.765625" customWidth="1"/>
-    <col min="9" max="9" width="9.23046875" style="11"/>
+    <col min="7" max="7" width="12.4609375" style="11" customWidth="1"/>
+    <col min="8" max="8" width="16.3828125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="18.23046875" style="11" customWidth="1"/>
+    <col min="10" max="10" width="15.3828125" style="11" customWidth="1"/>
+    <col min="11" max="14" width="2.15234375" style="11" customWidth="1"/>
+    <col min="15" max="15" width="13" customWidth="1"/>
+    <col min="16" max="16" width="14.765625" customWidth="1"/>
+    <col min="17" max="17" width="9.23046875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1">
-      <c r="A1" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="22"/>
+    <row r="1" spans="1:17" s="4" customFormat="1">
+      <c r="A1" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="21"/>
       <c r="C1" s="10"/>
-      <c r="D1" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="23"/>
+      <c r="D1" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="27"/>
       <c r="F1" s="11"/>
-      <c r="G1" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="11"/>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="G1" s="29"/>
+      <c r="H1" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="11"/>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B2" s="5">
         <v>0</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="16.3" customHeight="1">
-      <c r="A3" s="25" t="s">
-        <v>55</v>
+        <v>50</v>
+      </c>
+      <c r="E2" s="20">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="O2" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="16.3" customHeight="1">
+      <c r="A3" s="24" t="s">
+        <v>51</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="15">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3">
+        <v>75</v>
+      </c>
+      <c r="E3" s="26">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="O3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:17">
       <c r="A4" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B4" s="5">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="5">
+        <v>37</v>
+      </c>
+      <c r="E4" s="26">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>63</v>
-      </c>
-      <c r="H4">
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="O4" t="s">
+        <v>57</v>
+      </c>
+      <c r="P4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:17">
       <c r="A5" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B5" s="5">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="5">
-        <v>3</v>
-      </c>
-      <c r="G5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5">
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="O5" t="s">
+        <v>58</v>
+      </c>
+      <c r="P5">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:17">
       <c r="A6" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B6" s="5">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="5">
-        <v>4</v>
-      </c>
-      <c r="G6" t="s">
-        <v>65</v>
-      </c>
-      <c r="H6">
+        <v>7</v>
+      </c>
+      <c r="E6" s="26">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="O6" t="s">
+        <v>59</v>
+      </c>
+      <c r="P6">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:17">
       <c r="A7" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B7" s="5">
         <v>5</v>
       </c>
-      <c r="G7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H7">
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="20">
+        <v>2</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="O7" t="s">
+        <v>60</v>
+      </c>
+      <c r="P7">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:17">
       <c r="A8" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B8" s="5">
         <v>6</v>
       </c>
-      <c r="G8" t="s">
-        <v>67</v>
-      </c>
-      <c r="H8">
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="20">
+        <v>3</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="O8" t="s">
+        <v>61</v>
+      </c>
+      <c r="P8">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="G9" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9">
+    <row r="9" spans="1:17">
+      <c r="A9" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="5">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="20">
+        <v>4</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="O9" t="s">
+        <v>62</v>
+      </c>
+      <c r="P9">
         <v>128</v>
       </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>